<commit_message>
update files for January 2025
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_a_cy_monthly_overview.xlsx
+++ b/statistics_files/2025/2025_99_a_cy_monthly_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99A14E7-890B-4DC9-B3E9-6587F371223D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3045459E-EBBD-44A0-A5FA-03FC222D3E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="872" firstSheet="1" activeTab="28" xr2:uid="{6DE01D01-D2C0-4362-AEEE-36DB0900D2F9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="872" xr2:uid="{6DE01D01-D2C0-4362-AEEE-36DB0900D2F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Year total" sheetId="1" r:id="rId1"/>
@@ -2342,7 +2342,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:XFD1"/>
       <selection pane="topRight" sqref="A1:XFD1"/>
@@ -60896,7 +60896,7 @@
       <selection sqref="A1:XFD1"/>
       <selection pane="topRight" sqref="A1:XFD1"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61895,7 +61895,7 @@
   <sheetPr codeName="Sheet29"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:XFD1"/>
       <selection pane="topRight" sqref="A1:XFD1"/>

</xml_diff>